<commit_message>
Tamaño de borde adaptativo al width
</commit_message>
<xml_diff>
--- a/public/plantilla_importacion.xlsx
+++ b/public/plantilla_importacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nomec\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WWW\qrclean\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24966714-0A6B-40C4-9A76-E31052C8B2E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9627D2B-463C-42F0-886C-AA5E301FA5A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{CD99FFC8-766D-4F4F-BEC4-711670FC9A70}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="43200" windowHeight="23535" xr2:uid="{CD99FFC8-766D-4F4F-BEC4-711670FC9A70}"/>
   </bookViews>
   <sheets>
     <sheet name="PUESTOS" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>COD_PUESTO</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>FOTO</t>
+  </si>
+  <si>
+    <t>EMAIL USUARIO ASIGNADO</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B74C4C-5C2B-4427-861F-32955E8C8216}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,9 +445,10 @@
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,6 +466,9 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -473,7 +480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A886E45E-D973-4BCD-916D-28F2EABB4B79}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Estados de incidencia Encuestas Fase 1
</commit_message>
<xml_diff>
--- a/public/plantilla_importacion.xlsx
+++ b/public/plantilla_importacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WWW\qrclean\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9627D2B-463C-42F0-886C-AA5E301FA5A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2908899C-CEC1-494A-8108-A6AC64B644BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="43200" windowHeight="23535" xr2:uid="{CD99FFC8-766D-4F4F-BEC4-711670FC9A70}"/>
+    <workbookView xWindow="7800" yWindow="9870" windowWidth="43200" windowHeight="21465" xr2:uid="{CD99FFC8-766D-4F4F-BEC4-711670FC9A70}"/>
   </bookViews>
   <sheets>
     <sheet name="PUESTOS" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,6 +472,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E2572 F2:F1583" xr:uid="{F9B26812-57FC-4C3E-B24A-C288CB330E74}">
+      <formula1>"SI,NO"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Exportacion de QR en excel Posibilidad de actualizacion en la importacion de puestos Traduccion de cadenas de calendarios a español
</commit_message>
<xml_diff>
--- a/public/plantilla_importacion.xlsx
+++ b/public/plantilla_importacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WWW\qrclean\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2908899C-CEC1-494A-8108-A6AC64B644BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C71CD09-3252-4DFB-BF64-9651D9AEAF7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="9870" windowWidth="43200" windowHeight="21465" xr2:uid="{CD99FFC8-766D-4F4F-BEC4-711670FC9A70}"/>
+    <workbookView xWindow="7410" yWindow="7410" windowWidth="43200" windowHeight="23535" xr2:uid="{CD99FFC8-766D-4F4F-BEC4-711670FC9A70}"/>
   </bookViews>
   <sheets>
     <sheet name="PUESTOS" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>COD_PUESTO</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>EMAIL USUARIO ASIGNADO</t>
+  </si>
+  <si>
+    <t>ACTUALIZ</t>
   </si>
 </sst>
 </file>
@@ -431,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B74C4C-5C2B-4427-861F-32955E8C8216}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,9 +449,10 @@
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,11 +473,14 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E2572 F2:F1583" xr:uid="{F9B26812-57FC-4C3E-B24A-C288CB330E74}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E2572 F2:F1583 H2:H1583" xr:uid="{F9B26812-57FC-4C3E-B24A-C288CB330E74}">
       <formula1>"SI,NO"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>